<commit_message>
[Modify] D42011/ W42011/ template 42011 by Lukas
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/42011.xlsx
+++ b/PhoenixCI/Excel_Template/42011.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Bdc\結算部\風管組\個人資料區\CL.郭劻祥\1.測試\107年測試\107.1盤後子系統樣板升級\Excel_Template\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIN\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="120" windowWidth="14430" windowHeight="11085"/>
+    <workbookView xWindow="4716" yWindow="120" windowWidth="14436" windowHeight="11088"/>
   </bookViews>
   <sheets>
     <sheet name="保證金調整檢核表" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <r>
       <rPr>
@@ -323,19 +323,6 @@
       </rPr>
       <t>本日風險價格
 係數平均值</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>保證金
-所屬級距</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1495,7 +1482,26 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>所在級距與現行保證金所屬級距不同時，</t>
+      <t>所在級距與現行保證金所屬級距不同，且本日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>天期風險價格係數所屬級距與現行保證金所屬級距不同時，</t>
     </r>
     <r>
       <rPr>
@@ -1564,22 +1570,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>現行</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>保證金所屬級距</t>
+      <t>現行保證金所屬級距</t>
     </r>
     <r>
       <rPr>
@@ -1593,22 +1589,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>現行</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>保證金所屬級距</t>
+      <t>現行保證金所屬級距</t>
     </r>
     <r>
       <rPr>
@@ -1632,20 +1618,11 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>%</t>
+      <t>10%</t>
     </r>
     <r>
       <rPr>
@@ -1731,7 +1708,26 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>所在級距與現行保證金所屬級距不同之股票期貨</t>
+      <t>所在級距與現行保證金所屬級距不同，且本日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>天期風險價格係數所屬級距與現行保證金所屬級距不同之股票期貨</t>
     </r>
     <r>
       <rPr>
@@ -1780,6 +1776,16 @@
       </rPr>
       <t>)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現行保證金
+所屬級距</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現行保證金
+所屬級距</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2236,7 +2242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2501,8 +2507,11 @@
     <xf numFmtId="178" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2513,37 +2522,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2551,6 +2533,12 @@
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2564,7 +2552,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="31" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2572,6 +2572,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2585,13 +2594,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2604,6 +2610,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2914,199 +2923,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S938"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A289" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="O630" sqref="O630"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="5" customWidth="1"/>
-    <col min="8" max="9" width="15.5" style="5" customWidth="1"/>
-    <col min="10" max="13" width="13.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="5" customWidth="1"/>
-    <col min="16" max="18" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="15.44140625" style="5" customWidth="1"/>
+    <col min="10" max="13" width="13.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="5" customWidth="1"/>
+    <col min="16" max="18" width="13.6640625" style="2" customWidth="1"/>
     <col min="19" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.95" customHeight="1">
+    <row r="1" spans="1:19" ht="18.899999999999999" customHeight="1">
       <c r="O1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="110">
+      <c r="P1" s="108">
         <v>40596</v>
       </c>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109"/>
     </row>
     <row r="2" spans="1:19" ht="18" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
     </row>
     <row r="3" spans="1:19" ht="49.5" customHeight="1">
       <c r="B3" s="72">
         <v>1</v>
       </c>
-      <c r="C3" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
+      <c r="C3" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
     </row>
     <row r="4" spans="1:19" ht="51.75" customHeight="1">
       <c r="B4" s="72">
         <v>2</v>
       </c>
-      <c r="C4" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
+      <c r="C4" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
     </row>
     <row r="6" spans="1:19" ht="18" customHeight="1">
       <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1">
       <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
+      <c r="C7" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
     </row>
     <row r="8" spans="1:19" ht="39.75" customHeight="1">
       <c r="B8" s="13">
         <v>6</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
     </row>
     <row r="9" spans="1:19" ht="18" customHeight="1">
       <c r="B9" s="13"/>
@@ -3139,25 +3148,25 @@
       <c r="B11" s="73">
         <v>1</v>
       </c>
-      <c r="C11" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
+      <c r="C11" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
@@ -3173,112 +3182,112 @@
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="103" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="112" t="s">
+      <c r="D13" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="106" t="s">
+      <c r="F13" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="108"/>
-      <c r="L13" s="97" t="s">
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="99"/>
-      <c r="R13" s="115" t="s">
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="99"/>
+      <c r="S13" s="112"/>
     </row>
     <row r="14" spans="1:19" ht="18" customHeight="1">
-      <c r="B14" s="96"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="94"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="105" t="s">
+      <c r="D14" s="96"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="99" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="116" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="94" t="s">
+      <c r="I14" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="113" t="s">
+      <c r="L14" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="96" t="s">
+      <c r="M14" s="94"/>
+      <c r="N14" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="94"/>
-      <c r="N14" s="92" t="s">
+      <c r="O14" s="89"/>
+      <c r="P14" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="92"/>
-      <c r="P14" s="92" t="s">
+      <c r="Q14" s="88"/>
+      <c r="R14" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="118" t="s">
+      <c r="S14" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="93" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="15" spans="1:19" ht="18" customHeight="1">
-      <c r="B15" s="96"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="94"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="105"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="99"/>
       <c r="H15" s="94"/>
-      <c r="I15" s="117"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="94"/>
-      <c r="K15" s="113"/>
+      <c r="K15" s="114"/>
       <c r="L15" s="54" t="s">
         <v>3</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N15" s="67" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P15" s="67" t="s">
         <v>3</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="118"/>
-      <c r="S15" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="R15" s="106"/>
+      <c r="S15" s="88"/>
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="11"/>
@@ -10182,25 +10191,25 @@
     </row>
     <row r="316" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A316" s="11"/>
-      <c r="B316" s="101" t="s">
-        <v>34</v>
-      </c>
-      <c r="C316" s="101"/>
-      <c r="D316" s="101"/>
-      <c r="E316" s="101"/>
-      <c r="F316" s="101"/>
-      <c r="G316" s="101"/>
-      <c r="H316" s="101"/>
-      <c r="I316" s="101"/>
-      <c r="J316" s="101"/>
-      <c r="K316" s="101"/>
-      <c r="L316" s="101"/>
-      <c r="M316" s="101"/>
-      <c r="N316" s="101"/>
-      <c r="O316" s="101"/>
-      <c r="P316" s="101"/>
-      <c r="Q316" s="101"/>
-      <c r="R316" s="101"/>
+      <c r="B316" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="C316" s="117"/>
+      <c r="D316" s="117"/>
+      <c r="E316" s="117"/>
+      <c r="F316" s="117"/>
+      <c r="G316" s="117"/>
+      <c r="H316" s="117"/>
+      <c r="I316" s="117"/>
+      <c r="J316" s="117"/>
+      <c r="K316" s="117"/>
+      <c r="L316" s="117"/>
+      <c r="M316" s="117"/>
+      <c r="N316" s="117"/>
+      <c r="O316" s="117"/>
+      <c r="P316" s="117"/>
+      <c r="Q316" s="117"/>
+      <c r="R316" s="117"/>
     </row>
     <row r="317" spans="1:19" ht="18" customHeight="1"/>
     <row r="318" spans="1:19" s="2" customFormat="1" ht="50.25" customHeight="1">
@@ -10208,24 +10217,24 @@
       <c r="B318" s="73">
         <v>2</v>
       </c>
-      <c r="C318" s="100" t="s">
-        <v>38</v>
-      </c>
-      <c r="D318" s="100"/>
-      <c r="E318" s="100"/>
-      <c r="F318" s="100"/>
-      <c r="G318" s="100"/>
-      <c r="H318" s="100"/>
-      <c r="I318" s="100"/>
-      <c r="J318" s="100"/>
-      <c r="K318" s="100"/>
-      <c r="L318" s="100"/>
-      <c r="M318" s="100"/>
-      <c r="N318" s="100"/>
-      <c r="O318" s="100"/>
-      <c r="P318" s="100"/>
-      <c r="Q318" s="100"/>
-      <c r="R318" s="100"/>
+      <c r="C318" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="D318" s="98"/>
+      <c r="E318" s="98"/>
+      <c r="F318" s="98"/>
+      <c r="G318" s="98"/>
+      <c r="H318" s="98"/>
+      <c r="I318" s="98"/>
+      <c r="J318" s="98"/>
+      <c r="K318" s="98"/>
+      <c r="L318" s="98"/>
+      <c r="M318" s="98"/>
+      <c r="N318" s="98"/>
+      <c r="O318" s="98"/>
+      <c r="P318" s="98"/>
+      <c r="Q318" s="98"/>
+      <c r="R318" s="98"/>
     </row>
     <row r="319" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A319" s="1"/>
@@ -10241,112 +10250,112 @@
     </row>
     <row r="320" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A320" s="1"/>
-      <c r="B320" s="109" t="s">
+      <c r="B320" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C320" s="102" t="s">
+      <c r="C320" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D320" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="E320" s="112" t="s">
+      <c r="D320" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="E320" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F320" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G320" s="106" t="s">
+      <c r="F320" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G320" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="H320" s="107"/>
-      <c r="I320" s="107"/>
-      <c r="J320" s="107"/>
-      <c r="K320" s="108"/>
-      <c r="L320" s="97" t="s">
+      <c r="H320" s="101"/>
+      <c r="I320" s="101"/>
+      <c r="J320" s="101"/>
+      <c r="K320" s="102"/>
+      <c r="L320" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="M320" s="98"/>
-      <c r="N320" s="98"/>
-      <c r="O320" s="98"/>
-      <c r="P320" s="98"/>
-      <c r="Q320" s="99"/>
-      <c r="R320" s="115" t="s">
+      <c r="M320" s="111"/>
+      <c r="N320" s="111"/>
+      <c r="O320" s="111"/>
+      <c r="P320" s="111"/>
+      <c r="Q320" s="112"/>
+      <c r="R320" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="S320" s="99"/>
+      <c r="S320" s="112"/>
     </row>
     <row r="321" spans="1:19" ht="18" customHeight="1">
-      <c r="B321" s="96"/>
+      <c r="B321" s="97"/>
       <c r="C321" s="94"/>
-      <c r="D321" s="104"/>
-      <c r="E321" s="113"/>
-      <c r="F321" s="90"/>
+      <c r="D321" s="96"/>
+      <c r="E321" s="114"/>
+      <c r="F321" s="91"/>
       <c r="G321" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="H321" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="H321" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="I321" s="116" t="s">
-        <v>47</v>
-      </c>
-      <c r="J321" s="94" t="s">
+      <c r="I321" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="J321" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="K321" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="K321" s="113" t="s">
+      <c r="L321" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="L321" s="96" t="s">
+      <c r="M321" s="94"/>
+      <c r="N321" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="M321" s="94"/>
-      <c r="N321" s="92" t="s">
+      <c r="O321" s="89"/>
+      <c r="P321" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="O321" s="92"/>
-      <c r="P321" s="92" t="s">
+      <c r="Q321" s="88"/>
+      <c r="R321" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="Q321" s="93"/>
-      <c r="R321" s="118" t="s">
+      <c r="S321" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="S321" s="93" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="322" spans="1:19" ht="18" customHeight="1">
-      <c r="B322" s="96"/>
+      <c r="B322" s="97"/>
       <c r="C322" s="94"/>
-      <c r="D322" s="104"/>
-      <c r="E322" s="113"/>
-      <c r="F322" s="91"/>
-      <c r="G322" s="105"/>
+      <c r="D322" s="96"/>
+      <c r="E322" s="114"/>
+      <c r="F322" s="92"/>
+      <c r="G322" s="99"/>
       <c r="H322" s="94"/>
-      <c r="I322" s="117"/>
+      <c r="I322" s="105"/>
       <c r="J322" s="94"/>
-      <c r="K322" s="113"/>
+      <c r="K322" s="114"/>
       <c r="L322" s="54" t="s">
         <v>3</v>
       </c>
       <c r="M322" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N322" s="67" t="s">
         <v>3</v>
       </c>
       <c r="O322" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P322" s="67" t="s">
         <v>3</v>
       </c>
       <c r="Q322" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="R322" s="118"/>
-      <c r="S322" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="R322" s="106"/>
+      <c r="S322" s="88"/>
     </row>
     <row r="323" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A323" s="11"/>
@@ -17249,49 +17258,49 @@
       <c r="S622" s="27"/>
     </row>
     <row r="623" spans="1:19" ht="18" customHeight="1">
-      <c r="B623" s="101" t="s">
-        <v>35</v>
-      </c>
-      <c r="C623" s="101"/>
-      <c r="D623" s="101"/>
-      <c r="E623" s="101"/>
-      <c r="F623" s="101"/>
-      <c r="G623" s="101"/>
-      <c r="H623" s="101"/>
-      <c r="I623" s="101"/>
-      <c r="J623" s="101"/>
-      <c r="K623" s="101"/>
-      <c r="L623" s="101"/>
-      <c r="M623" s="101"/>
-      <c r="N623" s="101"/>
-      <c r="O623" s="101"/>
-      <c r="P623" s="101"/>
-      <c r="Q623" s="101"/>
-      <c r="R623" s="101"/>
+      <c r="B623" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="C623" s="117"/>
+      <c r="D623" s="117"/>
+      <c r="E623" s="117"/>
+      <c r="F623" s="117"/>
+      <c r="G623" s="117"/>
+      <c r="H623" s="117"/>
+      <c r="I623" s="117"/>
+      <c r="J623" s="117"/>
+      <c r="K623" s="117"/>
+      <c r="L623" s="117"/>
+      <c r="M623" s="117"/>
+      <c r="N623" s="117"/>
+      <c r="O623" s="117"/>
+      <c r="P623" s="117"/>
+      <c r="Q623" s="117"/>
+      <c r="R623" s="117"/>
     </row>
     <row r="624" spans="1:19" ht="18" customHeight="1"/>
     <row r="625" spans="2:19" ht="18" customHeight="1">
       <c r="B625" s="14">
         <v>3</v>
       </c>
-      <c r="C625" s="114" t="s">
-        <v>28</v>
-      </c>
-      <c r="D625" s="114"/>
-      <c r="E625" s="114"/>
-      <c r="F625" s="114"/>
-      <c r="G625" s="114"/>
-      <c r="H625" s="114"/>
-      <c r="I625" s="114"/>
-      <c r="J625" s="114"/>
-      <c r="K625" s="114"/>
-      <c r="L625" s="114"/>
-      <c r="M625" s="114"/>
-      <c r="N625" s="114"/>
-      <c r="O625" s="114"/>
-      <c r="P625" s="114"/>
-      <c r="Q625" s="114"/>
-      <c r="R625" s="114"/>
+      <c r="C625" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="D625" s="115"/>
+      <c r="E625" s="115"/>
+      <c r="F625" s="115"/>
+      <c r="G625" s="115"/>
+      <c r="H625" s="115"/>
+      <c r="I625" s="115"/>
+      <c r="J625" s="115"/>
+      <c r="K625" s="115"/>
+      <c r="L625" s="115"/>
+      <c r="M625" s="115"/>
+      <c r="N625" s="115"/>
+      <c r="O625" s="115"/>
+      <c r="P625" s="115"/>
+      <c r="Q625" s="115"/>
+      <c r="R625" s="115"/>
     </row>
     <row r="626" spans="2:19" ht="18" customHeight="1" thickBot="1">
       <c r="B626" s="14"/>
@@ -17300,105 +17309,105 @@
       </c>
     </row>
     <row r="627" spans="2:19" ht="18" customHeight="1">
-      <c r="B627" s="109" t="s">
+      <c r="B627" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C627" s="102" t="s">
+      <c r="C627" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D627" s="103" t="s">
-        <v>32</v>
-      </c>
-      <c r="E627" s="112" t="s">
+      <c r="D627" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="E627" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F627" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G627" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="H627" s="98"/>
-      <c r="I627" s="98"/>
-      <c r="J627" s="98"/>
-      <c r="K627" s="98"/>
-      <c r="L627" s="99"/>
-      <c r="M627" s="97" t="s">
+      <c r="F627" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G627" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="H627" s="111"/>
+      <c r="I627" s="111"/>
+      <c r="J627" s="111"/>
+      <c r="K627" s="111"/>
+      <c r="L627" s="112"/>
+      <c r="M627" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="N627" s="98"/>
-      <c r="O627" s="99"/>
-      <c r="P627" s="115" t="s">
+      <c r="N627" s="111"/>
+      <c r="O627" s="112"/>
+      <c r="P627" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="Q627" s="99"/>
+      <c r="Q627" s="112"/>
       <c r="R627" s="15"/>
     </row>
     <row r="628" spans="2:19" ht="18" customHeight="1">
-      <c r="B628" s="96"/>
+      <c r="B628" s="97"/>
       <c r="C628" s="94"/>
-      <c r="D628" s="104"/>
-      <c r="E628" s="113"/>
-      <c r="F628" s="90"/>
-      <c r="G628" s="96" t="s">
+      <c r="D628" s="96"/>
+      <c r="E628" s="114"/>
+      <c r="F628" s="91"/>
+      <c r="G628" s="97" t="s">
+        <v>20</v>
+      </c>
+      <c r="H628" s="94"/>
+      <c r="I628" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="H628" s="94"/>
-      <c r="I628" s="92" t="s">
+      <c r="J628" s="89"/>
+      <c r="K628" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="J628" s="92"/>
-      <c r="K628" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="L628" s="93"/>
-      <c r="M628" s="96" t="s">
+      <c r="L628" s="88"/>
+      <c r="M628" s="97" t="s">
         <v>17</v>
       </c>
       <c r="N628" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="O628" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="P628" s="118" t="s">
+      <c r="O628" s="123" t="s">
+        <v>50</v>
+      </c>
+      <c r="P628" s="106" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q628" s="88" t="s">
         <v>24</v>
-      </c>
-      <c r="Q628" s="93" t="s">
-        <v>25</v>
       </c>
       <c r="R628" s="3"/>
       <c r="S628" s="2"/>
     </row>
     <row r="629" spans="2:19" ht="18" customHeight="1">
-      <c r="B629" s="96"/>
+      <c r="B629" s="97"/>
       <c r="C629" s="94"/>
-      <c r="D629" s="104"/>
-      <c r="E629" s="113"/>
-      <c r="F629" s="91"/>
+      <c r="D629" s="96"/>
+      <c r="E629" s="114"/>
+      <c r="F629" s="92"/>
       <c r="G629" s="54" t="s">
         <v>3</v>
       </c>
       <c r="H629" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I629" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J629" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K629" s="67" t="s">
         <v>3</v>
       </c>
       <c r="L629" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="M629" s="96"/>
+        <v>25</v>
+      </c>
+      <c r="M629" s="97"/>
       <c r="N629" s="94"/>
-      <c r="O629" s="95"/>
-      <c r="P629" s="118"/>
-      <c r="Q629" s="93"/>
+      <c r="O629" s="107"/>
+      <c r="P629" s="106"/>
+      <c r="Q629" s="88"/>
       <c r="R629" s="3"/>
       <c r="S629" s="2"/>
     </row>
@@ -23443,19 +23452,17 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L320:Q320"/>
-    <mergeCell ref="B627:B629"/>
-    <mergeCell ref="I321:I322"/>
-    <mergeCell ref="G320:K320"/>
-    <mergeCell ref="H321:H322"/>
-    <mergeCell ref="J321:J322"/>
-    <mergeCell ref="K321:K322"/>
+    <mergeCell ref="R321:R322"/>
+    <mergeCell ref="P321:Q321"/>
+    <mergeCell ref="L13:Q13"/>
+    <mergeCell ref="C318:R318"/>
+    <mergeCell ref="B316:R316"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B320:B322"/>
     <mergeCell ref="C320:C322"/>
-    <mergeCell ref="R321:R322"/>
-    <mergeCell ref="P321:Q321"/>
     <mergeCell ref="G321:G322"/>
-    <mergeCell ref="N628:N629"/>
-    <mergeCell ref="P628:P629"/>
+    <mergeCell ref="E627:E629"/>
+    <mergeCell ref="G628:H628"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="M627:O627"/>
@@ -23470,8 +23477,8 @@
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="G627:L627"/>
     <mergeCell ref="B623:R623"/>
-    <mergeCell ref="E627:E629"/>
-    <mergeCell ref="M628:M629"/>
+    <mergeCell ref="B627:B629"/>
+    <mergeCell ref="I321:I322"/>
     <mergeCell ref="C5:R5"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D13:D15"/>
@@ -23483,21 +23490,23 @@
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="R14:R15"/>
     <mergeCell ref="C7:R7"/>
-    <mergeCell ref="F627:F629"/>
-    <mergeCell ref="K628:L628"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="O628:O629"/>
-    <mergeCell ref="G628:H628"/>
-    <mergeCell ref="L13:Q13"/>
-    <mergeCell ref="C318:R318"/>
-    <mergeCell ref="B316:R316"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="Q628:Q629"/>
     <mergeCell ref="N321:O321"/>
     <mergeCell ref="F320:F322"/>
     <mergeCell ref="I628:J628"/>
     <mergeCell ref="C627:C629"/>
     <mergeCell ref="D627:D629"/>
+    <mergeCell ref="M628:M629"/>
+    <mergeCell ref="F627:F629"/>
+    <mergeCell ref="K628:L628"/>
+    <mergeCell ref="O628:O629"/>
+    <mergeCell ref="N628:N629"/>
+    <mergeCell ref="P628:P629"/>
+    <mergeCell ref="G320:K320"/>
+    <mergeCell ref="H321:H322"/>
+    <mergeCell ref="J321:J322"/>
+    <mergeCell ref="K321:K322"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -23519,11 +23528,11 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="8" max="8" width="9.75" customWidth="1"/>
-    <col min="9" max="9" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -23531,18 +23540,18 @@
         <v>13</v>
       </c>
       <c r="C2" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="121" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="121" t="s">
-        <v>40</v>
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="121" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="121"/>
       <c r="H2" s="121" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="121"/>
     </row>
@@ -23550,20 +23559,20 @@
       <c r="B3" s="120"/>
       <c r="C3" s="120"/>
       <c r="D3" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="F3" s="120" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="120" t="s">
-        <v>45</v>
       </c>
       <c r="G3" s="120"/>
       <c r="H3" s="122" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="122" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="35.25" customHeight="1">
@@ -23575,7 +23584,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="122"/>
       <c r="I4" s="122"/>

</xml_diff>

<commit_message>
[Modify] 42011 template, W42011 by Lukas
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/42011.xlsx
+++ b/PhoenixCI/Excel_Template/42011.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Bdc\結算部\風管組\個人資料區\CL.郭劻祥\1.測試\107年測試\107.1盤後子系統樣板升級\Excel_Template\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIN\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="120" windowWidth="14430" windowHeight="11085"/>
+    <workbookView xWindow="4716" yWindow="120" windowWidth="14436" windowHeight="11088"/>
   </bookViews>
   <sheets>
     <sheet name="保證金調整檢核表" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <r>
       <rPr>
@@ -323,19 +323,6 @@
       </rPr>
       <t>本日風險價格
 係數平均值</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>保證金
-所屬級距</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1495,7 +1482,26 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>所在級距與現行保證金所屬級距不同時，</t>
+      <t>所在級距與現行保證金所屬級距不同，且本日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>天期風險價格係數所屬級距與現行保證金所屬級距不同時，</t>
     </r>
     <r>
       <rPr>
@@ -1564,22 +1570,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>現行</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>保證金所屬級距</t>
+      <t>現行保證金所屬級距</t>
     </r>
     <r>
       <rPr>
@@ -1593,22 +1589,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>現行</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>保證金所屬級距</t>
+      <t>現行保證金所屬級距</t>
     </r>
     <r>
       <rPr>
@@ -1632,20 +1618,11 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>%</t>
+      <t>10%</t>
     </r>
     <r>
       <rPr>
@@ -1731,7 +1708,26 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>所在級距與現行保證金所屬級距不同之股票期貨</t>
+      <t>所在級距與現行保證金所屬級距不同，且本日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>天期風險價格係數所屬級距與現行保證金所屬級距不同之股票期貨</t>
     </r>
     <r>
       <rPr>
@@ -1780,6 +1776,16 @@
       </rPr>
       <t>)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現行保證金
+所屬級距</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現行保證金
+所屬級距</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2236,7 +2242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2501,8 +2507,11 @@
     <xf numFmtId="178" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2513,37 +2522,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2551,6 +2533,12 @@
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2564,7 +2552,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="31" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2572,6 +2572,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2585,13 +2594,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2604,6 +2610,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2914,199 +2923,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S938"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A289" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="O630" sqref="O630"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="5" customWidth="1"/>
-    <col min="8" max="9" width="15.5" style="5" customWidth="1"/>
-    <col min="10" max="13" width="13.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="5" customWidth="1"/>
-    <col min="16" max="18" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="15.44140625" style="5" customWidth="1"/>
+    <col min="10" max="13" width="13.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="5" customWidth="1"/>
+    <col min="16" max="18" width="13.6640625" style="2" customWidth="1"/>
     <col min="19" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.95" customHeight="1">
+    <row r="1" spans="1:19" ht="18.899999999999999" customHeight="1">
       <c r="O1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="110">
+      <c r="P1" s="108">
         <v>40596</v>
       </c>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109"/>
     </row>
     <row r="2" spans="1:19" ht="18" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
     </row>
     <row r="3" spans="1:19" ht="49.5" customHeight="1">
       <c r="B3" s="72">
         <v>1</v>
       </c>
-      <c r="C3" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
+      <c r="C3" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
     </row>
     <row r="4" spans="1:19" ht="51.75" customHeight="1">
       <c r="B4" s="72">
         <v>2</v>
       </c>
-      <c r="C4" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
+      <c r="C4" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1">
       <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
     </row>
     <row r="6" spans="1:19" ht="18" customHeight="1">
       <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1">
       <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
+      <c r="C7" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
     </row>
     <row r="8" spans="1:19" ht="39.75" customHeight="1">
       <c r="B8" s="13">
         <v>6</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
     </row>
     <row r="9" spans="1:19" ht="18" customHeight="1">
       <c r="B9" s="13"/>
@@ -3139,25 +3148,25 @@
       <c r="B11" s="73">
         <v>1</v>
       </c>
-      <c r="C11" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
+      <c r="C11" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
@@ -3173,112 +3182,112 @@
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="103" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="112" t="s">
+      <c r="D13" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="106" t="s">
+      <c r="F13" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="108"/>
-      <c r="L13" s="97" t="s">
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="99"/>
-      <c r="R13" s="115" t="s">
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="99"/>
+      <c r="S13" s="112"/>
     </row>
     <row r="14" spans="1:19" ht="18" customHeight="1">
-      <c r="B14" s="96"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="94"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="105" t="s">
+      <c r="D14" s="96"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="99" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="116" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="94" t="s">
+      <c r="I14" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="113" t="s">
+      <c r="L14" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="96" t="s">
+      <c r="M14" s="94"/>
+      <c r="N14" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="94"/>
-      <c r="N14" s="92" t="s">
+      <c r="O14" s="89"/>
+      <c r="P14" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="92"/>
-      <c r="P14" s="92" t="s">
+      <c r="Q14" s="88"/>
+      <c r="R14" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="118" t="s">
+      <c r="S14" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="93" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="15" spans="1:19" ht="18" customHeight="1">
-      <c r="B15" s="96"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="94"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="105"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="99"/>
       <c r="H15" s="94"/>
-      <c r="I15" s="117"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="94"/>
-      <c r="K15" s="113"/>
+      <c r="K15" s="114"/>
       <c r="L15" s="54" t="s">
         <v>3</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N15" s="67" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P15" s="67" t="s">
         <v>3</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="118"/>
-      <c r="S15" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="R15" s="106"/>
+      <c r="S15" s="88"/>
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="11"/>
@@ -10182,25 +10191,25 @@
     </row>
     <row r="316" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A316" s="11"/>
-      <c r="B316" s="101" t="s">
-        <v>34</v>
-      </c>
-      <c r="C316" s="101"/>
-      <c r="D316" s="101"/>
-      <c r="E316" s="101"/>
-      <c r="F316" s="101"/>
-      <c r="G316" s="101"/>
-      <c r="H316" s="101"/>
-      <c r="I316" s="101"/>
-      <c r="J316" s="101"/>
-      <c r="K316" s="101"/>
-      <c r="L316" s="101"/>
-      <c r="M316" s="101"/>
-      <c r="N316" s="101"/>
-      <c r="O316" s="101"/>
-      <c r="P316" s="101"/>
-      <c r="Q316" s="101"/>
-      <c r="R316" s="101"/>
+      <c r="B316" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="C316" s="117"/>
+      <c r="D316" s="117"/>
+      <c r="E316" s="117"/>
+      <c r="F316" s="117"/>
+      <c r="G316" s="117"/>
+      <c r="H316" s="117"/>
+      <c r="I316" s="117"/>
+      <c r="J316" s="117"/>
+      <c r="K316" s="117"/>
+      <c r="L316" s="117"/>
+      <c r="M316" s="117"/>
+      <c r="N316" s="117"/>
+      <c r="O316" s="117"/>
+      <c r="P316" s="117"/>
+      <c r="Q316" s="117"/>
+      <c r="R316" s="117"/>
     </row>
     <row r="317" spans="1:19" ht="18" customHeight="1"/>
     <row r="318" spans="1:19" s="2" customFormat="1" ht="50.25" customHeight="1">
@@ -10208,24 +10217,24 @@
       <c r="B318" s="73">
         <v>2</v>
       </c>
-      <c r="C318" s="100" t="s">
-        <v>38</v>
-      </c>
-      <c r="D318" s="100"/>
-      <c r="E318" s="100"/>
-      <c r="F318" s="100"/>
-      <c r="G318" s="100"/>
-      <c r="H318" s="100"/>
-      <c r="I318" s="100"/>
-      <c r="J318" s="100"/>
-      <c r="K318" s="100"/>
-      <c r="L318" s="100"/>
-      <c r="M318" s="100"/>
-      <c r="N318" s="100"/>
-      <c r="O318" s="100"/>
-      <c r="P318" s="100"/>
-      <c r="Q318" s="100"/>
-      <c r="R318" s="100"/>
+      <c r="C318" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="D318" s="98"/>
+      <c r="E318" s="98"/>
+      <c r="F318" s="98"/>
+      <c r="G318" s="98"/>
+      <c r="H318" s="98"/>
+      <c r="I318" s="98"/>
+      <c r="J318" s="98"/>
+      <c r="K318" s="98"/>
+      <c r="L318" s="98"/>
+      <c r="M318" s="98"/>
+      <c r="N318" s="98"/>
+      <c r="O318" s="98"/>
+      <c r="P318" s="98"/>
+      <c r="Q318" s="98"/>
+      <c r="R318" s="98"/>
     </row>
     <row r="319" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A319" s="1"/>
@@ -10241,112 +10250,112 @@
     </row>
     <row r="320" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A320" s="1"/>
-      <c r="B320" s="109" t="s">
+      <c r="B320" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C320" s="102" t="s">
+      <c r="C320" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D320" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="E320" s="112" t="s">
+      <c r="D320" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="E320" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F320" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G320" s="106" t="s">
+      <c r="F320" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G320" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="H320" s="107"/>
-      <c r="I320" s="107"/>
-      <c r="J320" s="107"/>
-      <c r="K320" s="108"/>
-      <c r="L320" s="97" t="s">
+      <c r="H320" s="101"/>
+      <c r="I320" s="101"/>
+      <c r="J320" s="101"/>
+      <c r="K320" s="102"/>
+      <c r="L320" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="M320" s="98"/>
-      <c r="N320" s="98"/>
-      <c r="O320" s="98"/>
-      <c r="P320" s="98"/>
-      <c r="Q320" s="99"/>
-      <c r="R320" s="115" t="s">
+      <c r="M320" s="111"/>
+      <c r="N320" s="111"/>
+      <c r="O320" s="111"/>
+      <c r="P320" s="111"/>
+      <c r="Q320" s="112"/>
+      <c r="R320" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="S320" s="99"/>
+      <c r="S320" s="112"/>
     </row>
     <row r="321" spans="1:19" ht="18" customHeight="1">
-      <c r="B321" s="96"/>
+      <c r="B321" s="97"/>
       <c r="C321" s="94"/>
-      <c r="D321" s="104"/>
-      <c r="E321" s="113"/>
-      <c r="F321" s="90"/>
+      <c r="D321" s="96"/>
+      <c r="E321" s="114"/>
+      <c r="F321" s="91"/>
       <c r="G321" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="H321" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="H321" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="I321" s="116" t="s">
-        <v>47</v>
-      </c>
-      <c r="J321" s="94" t="s">
+      <c r="I321" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="J321" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="K321" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="K321" s="113" t="s">
+      <c r="L321" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="L321" s="96" t="s">
+      <c r="M321" s="94"/>
+      <c r="N321" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="M321" s="94"/>
-      <c r="N321" s="92" t="s">
+      <c r="O321" s="89"/>
+      <c r="P321" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="O321" s="92"/>
-      <c r="P321" s="92" t="s">
+      <c r="Q321" s="88"/>
+      <c r="R321" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="Q321" s="93"/>
-      <c r="R321" s="118" t="s">
+      <c r="S321" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="S321" s="93" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="322" spans="1:19" ht="18" customHeight="1">
-      <c r="B322" s="96"/>
+      <c r="B322" s="97"/>
       <c r="C322" s="94"/>
-      <c r="D322" s="104"/>
-      <c r="E322" s="113"/>
-      <c r="F322" s="91"/>
-      <c r="G322" s="105"/>
+      <c r="D322" s="96"/>
+      <c r="E322" s="114"/>
+      <c r="F322" s="92"/>
+      <c r="G322" s="99"/>
       <c r="H322" s="94"/>
-      <c r="I322" s="117"/>
+      <c r="I322" s="105"/>
       <c r="J322" s="94"/>
-      <c r="K322" s="113"/>
+      <c r="K322" s="114"/>
       <c r="L322" s="54" t="s">
         <v>3</v>
       </c>
       <c r="M322" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N322" s="67" t="s">
         <v>3</v>
       </c>
       <c r="O322" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P322" s="67" t="s">
         <v>3</v>
       </c>
       <c r="Q322" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="R322" s="118"/>
-      <c r="S322" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="R322" s="106"/>
+      <c r="S322" s="88"/>
     </row>
     <row r="323" spans="1:19" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A323" s="11"/>
@@ -17249,49 +17258,49 @@
       <c r="S622" s="27"/>
     </row>
     <row r="623" spans="1:19" ht="18" customHeight="1">
-      <c r="B623" s="101" t="s">
-        <v>35</v>
-      </c>
-      <c r="C623" s="101"/>
-      <c r="D623" s="101"/>
-      <c r="E623" s="101"/>
-      <c r="F623" s="101"/>
-      <c r="G623" s="101"/>
-      <c r="H623" s="101"/>
-      <c r="I623" s="101"/>
-      <c r="J623" s="101"/>
-      <c r="K623" s="101"/>
-      <c r="L623" s="101"/>
-      <c r="M623" s="101"/>
-      <c r="N623" s="101"/>
-      <c r="O623" s="101"/>
-      <c r="P623" s="101"/>
-      <c r="Q623" s="101"/>
-      <c r="R623" s="101"/>
+      <c r="B623" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="C623" s="117"/>
+      <c r="D623" s="117"/>
+      <c r="E623" s="117"/>
+      <c r="F623" s="117"/>
+      <c r="G623" s="117"/>
+      <c r="H623" s="117"/>
+      <c r="I623" s="117"/>
+      <c r="J623" s="117"/>
+      <c r="K623" s="117"/>
+      <c r="L623" s="117"/>
+      <c r="M623" s="117"/>
+      <c r="N623" s="117"/>
+      <c r="O623" s="117"/>
+      <c r="P623" s="117"/>
+      <c r="Q623" s="117"/>
+      <c r="R623" s="117"/>
     </row>
     <row r="624" spans="1:19" ht="18" customHeight="1"/>
     <row r="625" spans="2:19" ht="18" customHeight="1">
       <c r="B625" s="14">
         <v>3</v>
       </c>
-      <c r="C625" s="114" t="s">
-        <v>28</v>
-      </c>
-      <c r="D625" s="114"/>
-      <c r="E625" s="114"/>
-      <c r="F625" s="114"/>
-      <c r="G625" s="114"/>
-      <c r="H625" s="114"/>
-      <c r="I625" s="114"/>
-      <c r="J625" s="114"/>
-      <c r="K625" s="114"/>
-      <c r="L625" s="114"/>
-      <c r="M625" s="114"/>
-      <c r="N625" s="114"/>
-      <c r="O625" s="114"/>
-      <c r="P625" s="114"/>
-      <c r="Q625" s="114"/>
-      <c r="R625" s="114"/>
+      <c r="C625" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="D625" s="115"/>
+      <c r="E625" s="115"/>
+      <c r="F625" s="115"/>
+      <c r="G625" s="115"/>
+      <c r="H625" s="115"/>
+      <c r="I625" s="115"/>
+      <c r="J625" s="115"/>
+      <c r="K625" s="115"/>
+      <c r="L625" s="115"/>
+      <c r="M625" s="115"/>
+      <c r="N625" s="115"/>
+      <c r="O625" s="115"/>
+      <c r="P625" s="115"/>
+      <c r="Q625" s="115"/>
+      <c r="R625" s="115"/>
     </row>
     <row r="626" spans="2:19" ht="18" customHeight="1" thickBot="1">
       <c r="B626" s="14"/>
@@ -17300,105 +17309,105 @@
       </c>
     </row>
     <row r="627" spans="2:19" ht="18" customHeight="1">
-      <c r="B627" s="109" t="s">
+      <c r="B627" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C627" s="102" t="s">
+      <c r="C627" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D627" s="103" t="s">
-        <v>32</v>
-      </c>
-      <c r="E627" s="112" t="s">
+      <c r="D627" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="E627" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="F627" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="G627" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="H627" s="98"/>
-      <c r="I627" s="98"/>
-      <c r="J627" s="98"/>
-      <c r="K627" s="98"/>
-      <c r="L627" s="99"/>
-      <c r="M627" s="97" t="s">
+      <c r="F627" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G627" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="H627" s="111"/>
+      <c r="I627" s="111"/>
+      <c r="J627" s="111"/>
+      <c r="K627" s="111"/>
+      <c r="L627" s="112"/>
+      <c r="M627" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="N627" s="98"/>
-      <c r="O627" s="99"/>
-      <c r="P627" s="115" t="s">
+      <c r="N627" s="111"/>
+      <c r="O627" s="112"/>
+      <c r="P627" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="Q627" s="99"/>
+      <c r="Q627" s="112"/>
       <c r="R627" s="15"/>
     </row>
     <row r="628" spans="2:19" ht="18" customHeight="1">
-      <c r="B628" s="96"/>
+      <c r="B628" s="97"/>
       <c r="C628" s="94"/>
-      <c r="D628" s="104"/>
-      <c r="E628" s="113"/>
-      <c r="F628" s="90"/>
-      <c r="G628" s="96" t="s">
+      <c r="D628" s="96"/>
+      <c r="E628" s="114"/>
+      <c r="F628" s="91"/>
+      <c r="G628" s="97" t="s">
+        <v>20</v>
+      </c>
+      <c r="H628" s="94"/>
+      <c r="I628" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="H628" s="94"/>
-      <c r="I628" s="92" t="s">
+      <c r="J628" s="89"/>
+      <c r="K628" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="J628" s="92"/>
-      <c r="K628" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="L628" s="93"/>
-      <c r="M628" s="96" t="s">
+      <c r="L628" s="88"/>
+      <c r="M628" s="97" t="s">
         <v>17</v>
       </c>
       <c r="N628" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="O628" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="P628" s="118" t="s">
+      <c r="O628" s="123" t="s">
+        <v>50</v>
+      </c>
+      <c r="P628" s="106" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q628" s="88" t="s">
         <v>24</v>
-      </c>
-      <c r="Q628" s="93" t="s">
-        <v>25</v>
       </c>
       <c r="R628" s="3"/>
       <c r="S628" s="2"/>
     </row>
     <row r="629" spans="2:19" ht="18" customHeight="1">
-      <c r="B629" s="96"/>
+      <c r="B629" s="97"/>
       <c r="C629" s="94"/>
-      <c r="D629" s="104"/>
-      <c r="E629" s="113"/>
-      <c r="F629" s="91"/>
+      <c r="D629" s="96"/>
+      <c r="E629" s="114"/>
+      <c r="F629" s="92"/>
       <c r="G629" s="54" t="s">
         <v>3</v>
       </c>
       <c r="H629" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I629" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J629" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K629" s="67" t="s">
         <v>3</v>
       </c>
       <c r="L629" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="M629" s="96"/>
+        <v>25</v>
+      </c>
+      <c r="M629" s="97"/>
       <c r="N629" s="94"/>
-      <c r="O629" s="95"/>
-      <c r="P629" s="118"/>
-      <c r="Q629" s="93"/>
+      <c r="O629" s="107"/>
+      <c r="P629" s="106"/>
+      <c r="Q629" s="88"/>
       <c r="R629" s="3"/>
       <c r="S629" s="2"/>
     </row>
@@ -23443,19 +23452,17 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L320:Q320"/>
-    <mergeCell ref="B627:B629"/>
-    <mergeCell ref="I321:I322"/>
-    <mergeCell ref="G320:K320"/>
-    <mergeCell ref="H321:H322"/>
-    <mergeCell ref="J321:J322"/>
-    <mergeCell ref="K321:K322"/>
+    <mergeCell ref="R321:R322"/>
+    <mergeCell ref="P321:Q321"/>
+    <mergeCell ref="L13:Q13"/>
+    <mergeCell ref="C318:R318"/>
+    <mergeCell ref="B316:R316"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B320:B322"/>
     <mergeCell ref="C320:C322"/>
-    <mergeCell ref="R321:R322"/>
-    <mergeCell ref="P321:Q321"/>
     <mergeCell ref="G321:G322"/>
-    <mergeCell ref="N628:N629"/>
-    <mergeCell ref="P628:P629"/>
+    <mergeCell ref="E627:E629"/>
+    <mergeCell ref="G628:H628"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="M627:O627"/>
@@ -23470,8 +23477,8 @@
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="G627:L627"/>
     <mergeCell ref="B623:R623"/>
-    <mergeCell ref="E627:E629"/>
-    <mergeCell ref="M628:M629"/>
+    <mergeCell ref="B627:B629"/>
+    <mergeCell ref="I321:I322"/>
     <mergeCell ref="C5:R5"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D13:D15"/>
@@ -23483,21 +23490,23 @@
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="R14:R15"/>
     <mergeCell ref="C7:R7"/>
-    <mergeCell ref="F627:F629"/>
-    <mergeCell ref="K628:L628"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="O628:O629"/>
-    <mergeCell ref="G628:H628"/>
-    <mergeCell ref="L13:Q13"/>
-    <mergeCell ref="C318:R318"/>
-    <mergeCell ref="B316:R316"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="Q628:Q629"/>
     <mergeCell ref="N321:O321"/>
     <mergeCell ref="F320:F322"/>
     <mergeCell ref="I628:J628"/>
     <mergeCell ref="C627:C629"/>
     <mergeCell ref="D627:D629"/>
+    <mergeCell ref="M628:M629"/>
+    <mergeCell ref="F627:F629"/>
+    <mergeCell ref="K628:L628"/>
+    <mergeCell ref="O628:O629"/>
+    <mergeCell ref="N628:N629"/>
+    <mergeCell ref="P628:P629"/>
+    <mergeCell ref="G320:K320"/>
+    <mergeCell ref="H321:H322"/>
+    <mergeCell ref="J321:J322"/>
+    <mergeCell ref="K321:K322"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -23519,11 +23528,11 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="8" max="8" width="9.75" customWidth="1"/>
-    <col min="9" max="9" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -23531,18 +23540,18 @@
         <v>13</v>
       </c>
       <c r="C2" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="121" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="121" t="s">
-        <v>40</v>
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="121" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="121"/>
       <c r="H2" s="121" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="121"/>
     </row>
@@ -23550,20 +23559,20 @@
       <c r="B3" s="120"/>
       <c r="C3" s="120"/>
       <c r="D3" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="F3" s="120" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="120" t="s">
-        <v>45</v>
       </c>
       <c r="G3" s="120"/>
       <c r="H3" s="122" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="122" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="35.25" customHeight="1">
@@ -23575,7 +23584,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="122"/>
       <c r="I4" s="122"/>

</xml_diff>